<commit_message>
Added OPAMPS in EAGLE SCH
</commit_message>
<xml_diff>
--- a/Parts/Parts.xlsx
+++ b/Parts/Parts.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>VALUE</t>
   </si>
@@ -73,12 +73,6 @@
     <t>LABEL(S)</t>
   </si>
   <si>
-    <t>R2,R4,R6</t>
-  </si>
-  <si>
-    <t>R3,R5</t>
-  </si>
-  <si>
     <t>R9,R12,R14</t>
   </si>
   <si>
@@ -95,6 +89,39 @@
   </si>
   <si>
     <t>100k</t>
+  </si>
+  <si>
+    <t>CAPACITOR</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>3.3uF</t>
+  </si>
+  <si>
+    <t>478-3866-1-ND</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>100uF</t>
+  </si>
+  <si>
+    <t>493-3852-1-ND</t>
+  </si>
+  <si>
+    <t>R2,R3,R4,R6</t>
+  </si>
+  <si>
+    <t>R5,R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>311-3.30KFRCT-ND</t>
   </si>
 </sst>
 </file>
@@ -178,13 +205,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -192,9 +222,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -230,6 +257,9 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -244,16 +274,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I12" totalsRowShown="0">
-  <autoFilter ref="B6:I12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I15" totalsRowShown="0">
+  <autoFilter ref="B6:I15"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ITEM"/>
     <tableColumn id="8" name="Schematic"/>
     <tableColumn id="2" name="LABEL(S)"/>
-    <tableColumn id="3" name="VALUE" dataDxfId="0"/>
+    <tableColumn id="3" name="VALUE" dataDxfId="3"/>
     <tableColumn id="4" name="Digikey "/>
     <tableColumn id="6" name="UNITS"/>
-    <tableColumn id="5" name="Price"/>
+    <tableColumn id="5" name="Price" dataCellStyle="Currency"/>
     <tableColumn id="7" name="COST" dataCellStyle="Currency">
       <calculatedColumnFormula>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</calculatedColumnFormula>
     </tableColumn>
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I12"/>
+  <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -541,11 +571,11 @@
   <sheetData>
     <row r="3" spans="2:9">
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I3" s="4">
         <f>SUM(Table1[COST])</f>
-        <v>8.43</v>
+        <v>10.23</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -553,7 +583,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -582,13 +612,16 @@
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7">
         <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
       </c>
       <c r="I7" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
@@ -600,7 +633,7 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -624,13 +657,16 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
       </c>
       <c r="I9" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
@@ -642,77 +678,160 @@
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>0.59</v>
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.1</v>
       </c>
       <c r="I10" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
-        <v>1.77</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="G11">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.59</v>
       </c>
       <c r="I11" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
-        <v>0</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1"/>
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
       <c r="I12" s="2">
         <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="2:9">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.34</v>
+      </c>
+      <c r="I14" s="8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.26</v>
+      </c>
+      <c r="I15" s="8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>1.26</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1"/>
-    <hyperlink ref="F10" r:id="rId2"/>
+    <hyperlink ref="F11" r:id="rId2"/>
     <hyperlink ref="F7" r:id="rId3"/>
+    <hyperlink ref="F14" r:id="rId4"/>
+    <hyperlink ref="F15" r:id="rId5"/>
+    <hyperlink ref="F10" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
sFPI - Rev 1
</commit_message>
<xml_diff>
--- a/Parts/Parts.xlsx
+++ b/Parts/Parts.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7760"/>
+    <workbookView xWindow="-80" yWindow="20" windowWidth="25580" windowHeight="15520"/>
   </bookViews>
   <sheets>
     <sheet name="Parts-Budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Schematic-sFPI-Driver" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>VALUE</t>
   </si>
@@ -122,6 +121,27 @@
   </si>
   <si>
     <t>311-3.30KFRCT-ND</t>
+  </si>
+  <si>
+    <t>Positive Adjustable Voltage Regulator</t>
+  </si>
+  <si>
+    <t>LT3080EST#TRPBFCT-ND</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>490-7516-1-ND</t>
+  </si>
+  <si>
+    <t>5M</t>
+  </si>
+  <si>
+    <t>SPRU505C-ND</t>
   </si>
 </sst>
 </file>
@@ -221,7 +241,42 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -274,13 +329,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I15" totalsRowShown="0">
-  <autoFilter ref="B6:I15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B6:I18" totalsRowShown="0">
+  <autoFilter ref="B6:I18"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ITEM"/>
     <tableColumn id="8" name="Schematic"/>
     <tableColumn id="2" name="LABEL(S)"/>
-    <tableColumn id="3" name="VALUE" dataDxfId="3"/>
+    <tableColumn id="3" name="VALUE" dataDxfId="6"/>
     <tableColumn id="4" name="Digikey "/>
     <tableColumn id="6" name="UNITS"/>
     <tableColumn id="5" name="Price" dataCellStyle="Currency"/>
@@ -555,15 +610,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I15"/>
+  <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="37.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
@@ -575,7 +631,7 @@
       </c>
       <c r="I3" s="4">
         <f>SUM(Table1[COST])</f>
-        <v>10.23</v>
+        <v>25.91</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -809,16 +865,85 @@
         <v>1.26</v>
       </c>
     </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4.22</v>
+      </c>
+      <c r="I16" s="8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="I17" s="8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8">
+        <v>10.64</v>
+      </c>
+      <c r="I18" s="8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[UNITS]]</f>
+        <v>10.64</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>20</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
-      <formula>30</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -828,10 +953,13 @@
     <hyperlink ref="F14" r:id="rId4"/>
     <hyperlink ref="F15" r:id="rId5"/>
     <hyperlink ref="F10" r:id="rId6"/>
+    <hyperlink ref="F16" r:id="rId7"/>
+    <hyperlink ref="F17" r:id="rId8"/>
+    <hyperlink ref="F18" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -839,23 +967,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="25" zoomScaleNormal="25" zoomScalePageLayoutView="25" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>